<commit_message>
Test adding noise to bounding box
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-8300" windowWidth="25600" windowHeight="14560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="25180" windowHeight="13780" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -781,11 +782,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2137228520"/>
-        <c:axId val="2132479624"/>
+        <c:axId val="2126284616"/>
+        <c:axId val="2126287752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2137228520"/>
+        <c:axId val="2126284616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -794,7 +795,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132479624"/>
+        <c:crossAx val="2126287752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -802,7 +803,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132479624"/>
+        <c:axId val="2126287752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -813,7 +814,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2137228520"/>
+        <c:crossAx val="2126284616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1153,11 +1154,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2136298232"/>
-        <c:axId val="2139972472"/>
+        <c:axId val="2126314184"/>
+        <c:axId val="2126317448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2136298232"/>
+        <c:axId val="2126314184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1176,7 +1177,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2139972472"/>
+        <c:crossAx val="2126317448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1184,7 +1185,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2139972472"/>
+        <c:axId val="2126317448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1229,7 +1230,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2136298232"/>
+        <c:crossAx val="2126314184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1579,11 +1580,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2141838328"/>
-        <c:axId val="2141813896"/>
+        <c:axId val="2128119160"/>
+        <c:axId val="2128122264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2141838328"/>
+        <c:axId val="2128119160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1602,7 +1603,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2141813896"/>
+        <c:crossAx val="2128122264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1610,7 +1611,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2141813896"/>
+        <c:axId val="2128122264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1655,7 +1656,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2141838328"/>
+        <c:crossAx val="2128119160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3244,8 +3245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3817,4 +3818,21 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>